<commit_message>
Updated demo/test import files
</commit_message>
<xml_diff>
--- a/DataFiles/REMS2020_Template_1_Information.xlsx
+++ b/DataFiles/REMS2020_Template_1_Information.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqmstow1\Documents\GitHub\REMS2020\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqmstow1\Documents\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="360" windowWidth="15480" windowHeight="9000" tabRatio="695"/>
+    <workbookView xWindow="240" yWindow="360" windowWidth="15480" windowHeight="9000" tabRatio="695" firstSheet="1" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="10" r:id="rId1"/>
@@ -654,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -676,6 +676,31 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -685,10 +710,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A2:A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -722,6 +747,26 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -732,10 +777,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -775,6 +820,26 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -785,10 +850,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -810,6 +875,26 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -819,10 +904,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -850,6 +935,38 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -859,7 +976,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
@@ -882,7 +999,25 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
       <c r="C2" s="9"/>
+    </row>
+    <row r="3" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -894,10 +1029,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -919,6 +1054,38 @@
         <v>14</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -926,10 +1093,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -948,6 +1115,26 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -958,10 +1145,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -992,6 +1179,70 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1001,10 +1252,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1044,6 +1295,94 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1053,10 +1392,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1075,6 +1414,26 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1084,10 +1443,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1109,6 +1468,26 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>